<commit_message>
agregue metodos primer parciall excel- Falta condicion
</commit_message>
<xml_diff>
--- a/Metodo Segundo Parcial/Metodo de Lagrange.xlsx
+++ b/Metodo Segundo Parcial/Metodo de Lagrange.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Analisis Numerico Git\Metodo Segundo Parcial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCA2526-FFA1-4A02-92BF-AE69D645FE03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E863300-F41C-4005-B436-70B1B72F5AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metodo de Lagrange" sheetId="1" r:id="rId1"/>
@@ -308,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -336,10 +336,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AE18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,8 +1138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD686C09-A263-43A7-8435-78F2617DBFF8}">
   <dimension ref="B2:R33"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12:R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,27 +1499,27 @@
         <v>3</v>
       </c>
       <c r="C21" s="6">
-        <f>F4*D4</f>
+        <f t="shared" ref="C21:C26" si="0">F4*D4</f>
         <v>-0.26666000000000001</v>
       </c>
       <c r="D21" s="6">
-        <f>G4*D4</f>
+        <f t="shared" ref="D21:D26" si="1">G4*D4</f>
         <v>2.6665999999999999</v>
       </c>
       <c r="E21" s="4">
-        <f>H4*D4</f>
+        <f t="shared" ref="E21:E26" si="2">H4*D4</f>
         <v>-10.333</v>
       </c>
       <c r="F21" s="4">
-        <f>I4*D4</f>
+        <f t="shared" ref="F21:F26" si="3">I4*D4</f>
         <v>19.333300000000001</v>
       </c>
       <c r="G21" s="4">
-        <f>J4*D4</f>
+        <f t="shared" ref="G21:G26" si="4">J4*D4</f>
         <v>-17.399999999999999</v>
       </c>
       <c r="H21" s="4">
-        <f>K4*D4</f>
+        <f t="shared" ref="H21:H26" si="5">K4*D4</f>
         <v>6</v>
       </c>
     </row>
@@ -1532,27 +1528,27 @@
         <v>4</v>
       </c>
       <c r="C22" s="6">
-        <f>F5*D5</f>
+        <f t="shared" si="0"/>
         <v>2.824627</v>
       </c>
       <c r="D22" s="6">
-        <f>G5*D5</f>
+        <f t="shared" si="1"/>
         <v>-26.840525400000004</v>
       </c>
       <c r="E22" s="4">
-        <f>H5*D5</f>
+        <f t="shared" si="2"/>
         <v>96.766254000000004</v>
       </c>
       <c r="F22" s="4">
-        <f>I5*D5</f>
+        <f t="shared" si="3"/>
         <v>-162.80976269999999</v>
       </c>
       <c r="G22" s="4">
-        <f>J5*D5</f>
+        <f t="shared" si="4"/>
         <v>123.96150000000002</v>
       </c>
       <c r="H22" s="4">
-        <f>K5*D5</f>
+        <f t="shared" si="5"/>
         <v>-31.785000000000004</v>
       </c>
     </row>
@@ -1561,27 +1557,27 @@
         <v>5</v>
       </c>
       <c r="C23" s="6">
-        <f>F6*D6</f>
+        <f t="shared" si="0"/>
         <v>-7.7580600000000004</v>
       </c>
       <c r="D23" s="6">
-        <f>G6*D6</f>
+        <f t="shared" si="1"/>
         <v>69.84</v>
       </c>
       <c r="E23" s="4">
-        <f>H6*D6</f>
+        <f t="shared" si="2"/>
         <v>-234.73805999999999</v>
       </c>
       <c r="F23" s="4">
-        <f>I6*D6</f>
+        <f t="shared" si="3"/>
         <v>360.84000000000003</v>
       </c>
       <c r="G23" s="4">
-        <f>J6*D6</f>
+        <f t="shared" si="4"/>
         <v>-246.37980600000003</v>
       </c>
       <c r="H23" s="4">
-        <f>K6*D6</f>
+        <f t="shared" si="5"/>
         <v>58.2</v>
       </c>
     </row>
@@ -1590,27 +1586,27 @@
         <v>6</v>
       </c>
       <c r="C24" s="6">
-        <f>F7*D7</f>
+        <f t="shared" si="0"/>
         <v>10.51737</v>
       </c>
       <c r="D24" s="6">
-        <f>G7*D7</f>
+        <f t="shared" si="1"/>
         <v>-89.417369999999991</v>
       </c>
       <c r="E24" s="4">
-        <f>H7*D7</f>
+        <f t="shared" si="2"/>
         <v>281.40986849999996</v>
       </c>
       <c r="F24" s="4">
-        <f>I7*D7</f>
+        <f t="shared" si="3"/>
         <v>-403.70486849999998</v>
       </c>
       <c r="G24" s="4">
-        <f>J7*D7</f>
+        <f t="shared" si="4"/>
         <v>260.37</v>
       </c>
       <c r="H24" s="4">
-        <f>K7*D7</f>
+        <f t="shared" si="5"/>
         <v>-59.174999999999997</v>
       </c>
     </row>
@@ -1619,27 +1615,27 @@
         <v>24</v>
       </c>
       <c r="C25" s="6">
-        <f>F8*D8</f>
+        <f t="shared" si="0"/>
         <v>-7.6264759999999994</v>
       </c>
       <c r="D25" s="6">
-        <f>G8*D8</f>
+        <f t="shared" si="1"/>
         <v>61.012951999999999</v>
       </c>
       <c r="E25" s="4">
-        <f>H8*D8</f>
+        <f t="shared" si="2"/>
         <v>-181.13295199999999</v>
       </c>
       <c r="F25" s="4">
-        <f>I8*D8</f>
+        <f t="shared" si="3"/>
         <v>247.86647600000001</v>
       </c>
       <c r="G25" s="4">
-        <f>J8*D8</f>
+        <f t="shared" si="4"/>
         <v>-154.44</v>
       </c>
       <c r="H25" s="4">
-        <f>K8*D8</f>
+        <f t="shared" si="5"/>
         <v>34.32</v>
       </c>
     </row>
@@ -1648,53 +1644,53 @@
         <v>25</v>
       </c>
       <c r="C26" s="6">
-        <f>F9*D9</f>
+        <f t="shared" si="0"/>
         <v>2.31866087</v>
       </c>
       <c r="D26" s="6">
-        <f>G9*D9</f>
+        <f t="shared" si="1"/>
         <v>-17.39</v>
       </c>
       <c r="E26" s="4">
-        <f>H9*D9</f>
+        <f t="shared" si="2"/>
         <v>49.271087000000001</v>
       </c>
       <c r="F26" s="4">
-        <f>I9*D9</f>
+        <f t="shared" si="3"/>
         <v>-65.212500000000006</v>
       </c>
       <c r="G26" s="4">
-        <f>J9*D9</f>
+        <f t="shared" si="4"/>
         <v>39.706587000000006</v>
       </c>
       <c r="H26" s="4">
-        <f>K9*D9</f>
+        <f t="shared" si="5"/>
         <v>-8.6950000000000003</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C27" s="14">
-        <f>SUM(C21:C26)</f>
+        <f t="shared" ref="C27:H27" si="6">SUM(C21:C26)</f>
         <v>9.4618699999995393E-3</v>
       </c>
       <c r="D27" s="14">
-        <f>SUM(D21:D26)</f>
+        <f t="shared" si="6"/>
         <v>-0.12834339999999145</v>
       </c>
       <c r="E27" s="12">
-        <f>SUM(E21:E26)</f>
+        <f t="shared" si="6"/>
         <v>1.2431974999999866</v>
       </c>
       <c r="F27" s="12">
-        <f>SUM(F21:F26)</f>
+        <f t="shared" si="6"/>
         <v>-3.6873551999999279</v>
       </c>
       <c r="G27" s="12">
-        <f>SUM(G21:G26)</f>
+        <f t="shared" si="6"/>
         <v>5.818281000000006</v>
       </c>
       <c r="H27" s="12">
-        <f>SUM(H21:H26)</f>
+        <f t="shared" si="6"/>
         <v>-1.134999999999998</v>
       </c>
     </row>
@@ -1728,8 +1724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA78DD5-4499-49F4-9240-1610E91FF97E}">
   <dimension ref="B2:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,19 +1951,16 @@
       <c r="M8" s="6"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="N12" s="13" t="s">
@@ -2024,14 +2017,7 @@
       <c r="Q16" s="13"/>
       <c r="R16" s="13"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C20" s="11"/>
       <c r="D20" s="11" t="s">
         <v>22</v>
@@ -2039,7 +2025,7 @@
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>3</v>
       </c>
@@ -2064,7 +2050,7 @@
         <v>21.375</v>
       </c>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>4</v>
       </c>
@@ -2089,7 +2075,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>5</v>
       </c>
@@ -2114,7 +2100,7 @@
         <v>26.25</v>
       </c>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>6</v>
       </c>
@@ -2139,7 +2125,7 @@
         <v>-29.625</v>
       </c>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>24</v>
       </c>
@@ -2164,8 +2150,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B26" s="15"/>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
       <c r="C26" s="14">
         <f>SUM(C21:C25)</f>
         <v>5.0000000000001155E-3</v>
@@ -2187,7 +2173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="I27" s="7" t="s">
         <v>62</v>
       </c>
@@ -2195,7 +2181,7 @@
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="I28" s="7" t="s">
         <v>64</v>
       </c>
@@ -2203,7 +2189,7 @@
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
         <v>19</v>
       </c>
@@ -2218,7 +2204,7 @@
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="s">
         <v>60</v>
       </c>
@@ -2233,7 +2219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F07C2DD-BF2F-45CB-9372-1F33BE6AFEA2}">
   <dimension ref="B2:T32"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -2644,31 +2630,31 @@
         <v>3</v>
       </c>
       <c r="C21" s="6">
-        <f>F4*D4</f>
+        <f t="shared" ref="C21:C27" si="0">F4*D4</f>
         <v>0</v>
       </c>
       <c r="D21" s="6">
-        <f>G4*D4</f>
+        <f t="shared" ref="D21:D27" si="1">G4*D4</f>
         <v>-13333</v>
       </c>
       <c r="E21" s="6">
-        <f>H4*D4</f>
+        <f t="shared" ref="E21:E27" si="2">H4*D4</f>
         <v>133330</v>
       </c>
       <c r="F21" s="4">
-        <f>I4*D4</f>
+        <f t="shared" ref="F21:F27" si="3">I4*D4</f>
         <v>-516650</v>
       </c>
       <c r="G21" s="4">
-        <f>J4*D4</f>
+        <f t="shared" ref="G21:G27" si="4">J4*D4</f>
         <v>966665.00000000012</v>
       </c>
       <c r="H21" s="4">
-        <f>K4*D4</f>
+        <f t="shared" ref="H21:H27" si="5">K4*D4</f>
         <v>-869999.99999999988</v>
       </c>
       <c r="I21" s="4">
-        <f>L4*D4</f>
+        <f t="shared" ref="I21:I27" si="6">L4*D4</f>
         <v>300000</v>
       </c>
     </row>
@@ -2677,31 +2663,31 @@
         <v>4</v>
       </c>
       <c r="C22" s="6">
-        <f>F5*D5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D22" s="6">
-        <f>G5*D5</f>
+        <f t="shared" si="1"/>
         <v>46655</v>
       </c>
       <c r="E22" s="6">
-        <f>H5*D5</f>
+        <f t="shared" si="2"/>
         <v>-443331</v>
       </c>
       <c r="F22" s="4">
-        <f>I5*D5</f>
+        <f t="shared" si="3"/>
         <v>1598310</v>
       </c>
       <c r="G22" s="4">
-        <f>J5*D5</f>
+        <f t="shared" si="4"/>
         <v>-2689165.5</v>
       </c>
       <c r="H22" s="4">
-        <f>K5*D5</f>
+        <f t="shared" si="5"/>
         <v>2047500</v>
       </c>
       <c r="I22" s="4">
-        <f>L5*D5</f>
+        <f t="shared" si="6"/>
         <v>-525000</v>
       </c>
     </row>
@@ -2710,31 +2696,31 @@
         <v>5</v>
       </c>
       <c r="C23" s="6">
-        <f>F6*D6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D23" s="6">
-        <f>G6*D6</f>
+        <f t="shared" si="1"/>
         <v>-82646</v>
       </c>
       <c r="E23" s="6">
-        <f>H6*D6</f>
+        <f t="shared" si="2"/>
         <v>744000</v>
       </c>
       <c r="F23" s="4">
-        <f>I6*D6</f>
+        <f t="shared" si="3"/>
         <v>-2500646</v>
       </c>
       <c r="G23" s="4">
-        <f>J6*D6</f>
+        <f t="shared" si="4"/>
         <v>3844000</v>
       </c>
       <c r="H23" s="4">
-        <f>K6*D6</f>
+        <f t="shared" si="5"/>
         <v>-2624664.6</v>
       </c>
       <c r="I23" s="4">
-        <f>L6*D6</f>
+        <f t="shared" si="6"/>
         <v>620000</v>
       </c>
     </row>
@@ -2743,31 +2729,31 @@
         <v>6</v>
       </c>
       <c r="C24" s="6">
-        <f>F7*D7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D24" s="6">
-        <f>G7*D7</f>
+        <f t="shared" si="1"/>
         <v>53320</v>
       </c>
       <c r="E24" s="6">
-        <f>H7*D7</f>
+        <f t="shared" si="2"/>
         <v>-453320</v>
       </c>
       <c r="F24" s="4">
-        <f>I7*D7</f>
+        <f t="shared" si="3"/>
         <v>1426665.9999999998</v>
       </c>
       <c r="G24" s="4">
-        <f>J7*D7</f>
+        <f t="shared" si="4"/>
         <v>-2046665.9999999998</v>
       </c>
       <c r="H24" s="4">
-        <f>K7*D7</f>
+        <f t="shared" si="5"/>
         <v>1320000</v>
       </c>
       <c r="I24" s="4">
-        <f>L7*D7</f>
+        <f t="shared" si="6"/>
         <v>-300000</v>
       </c>
     </row>
@@ -2776,31 +2762,31 @@
         <v>24</v>
       </c>
       <c r="C25" s="6">
-        <f>F8*D8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D25" s="6">
-        <f>G8*D8</f>
+        <f t="shared" si="1"/>
         <v>-25332.699999999997</v>
       </c>
       <c r="E25" s="6">
-        <f>H8*D8</f>
+        <f t="shared" si="2"/>
         <v>202665.40000000002</v>
       </c>
       <c r="F25" s="4">
-        <f>I8*D8</f>
+        <f t="shared" si="3"/>
         <v>-601665.4</v>
       </c>
       <c r="G25" s="4">
-        <f>J8*D8</f>
+        <f t="shared" si="4"/>
         <v>823332.70000000007</v>
       </c>
       <c r="H25" s="4">
-        <f>K8*D8</f>
+        <f t="shared" si="5"/>
         <v>-513000</v>
       </c>
       <c r="I25" s="4">
-        <f>L8*D8</f>
+        <f t="shared" si="6"/>
         <v>114000</v>
       </c>
     </row>
@@ -2809,31 +2795,31 @@
         <v>25</v>
       </c>
       <c r="C26" s="6">
-        <f>F9*D9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D26" s="6">
-        <f>G9*D9</f>
+        <f t="shared" si="1"/>
         <v>3199.9920000000002</v>
       </c>
       <c r="E26" s="6">
-        <f>H9*D9</f>
+        <f t="shared" si="2"/>
         <v>-24000</v>
       </c>
       <c r="F26" s="4">
-        <f>I9*D9</f>
+        <f t="shared" si="3"/>
         <v>67999.199999999997</v>
       </c>
       <c r="G26" s="4">
-        <f>J9*D9</f>
+        <f t="shared" si="4"/>
         <v>-90000</v>
       </c>
       <c r="H26" s="4">
-        <f>K9*D9</f>
+        <f t="shared" si="5"/>
         <v>54799.200000000004</v>
       </c>
       <c r="I26" s="4">
-        <f>L9*D9</f>
+        <f t="shared" si="6"/>
         <v>-12000</v>
       </c>
     </row>
@@ -2842,31 +2828,31 @@
         <v>47</v>
       </c>
       <c r="C27" s="6">
-        <f>F10*D10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D27" s="6">
-        <f>G10*D10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E27" s="6">
-        <f>H10*D10</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F27" s="4">
-        <f>I10*D10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G27" s="4">
-        <f>J10*D10</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H27" s="4">
-        <f>K10*D10</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I27" s="4">
-        <f>L10*D10</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2875,31 +2861,31 @@
         <v>56</v>
       </c>
       <c r="C28" s="6">
-        <f>SUM(C21:C27)</f>
+        <f t="shared" ref="C28:I28" si="7">SUM(C21:C27)</f>
         <v>0</v>
       </c>
       <c r="D28" s="14">
-        <f>SUM(D21:D27)</f>
+        <f t="shared" si="7"/>
         <v>-18136.707999999999</v>
       </c>
       <c r="E28" s="14">
-        <f>SUM(E21:E27)</f>
+        <f t="shared" si="7"/>
         <v>159344.40000000002</v>
       </c>
       <c r="F28" s="12">
-        <f>SUM(F21:F27)</f>
+        <f t="shared" si="7"/>
         <v>-525986.2000000003</v>
       </c>
       <c r="G28" s="12">
-        <f>SUM(G21:G27)</f>
+        <f t="shared" si="7"/>
         <v>808166.2000000003</v>
       </c>
       <c r="H28" s="12">
-        <f>SUM(H21:H27)</f>
+        <f t="shared" si="7"/>
         <v>-585365.40000000014</v>
       </c>
       <c r="I28" s="12">
-        <f>SUM(I21:I27)</f>
+        <f t="shared" si="7"/>
         <v>197000</v>
       </c>
     </row>

</xml_diff>